<commit_message>
now the inherit def is work like a charm
</commit_message>
<xml_diff>
--- a/tutorial7_io_plotting/data.xlsx
+++ b/tutorial7_io_plotting/data.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>